<commit_message>
add coop tin to registration
</commit_message>
<xml_diff>
--- a/db/uploads/vote_power.xlsx
+++ b/db/uploads/vote_power.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ansellgabrieldelayre/Sites/GA_system/db/uploads/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BDFBFAB2-981C-BD41-9F97-DE92C8ADEF74}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{373A93B1-4C48-2843-927B-F0C7B3BC7D62}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="760" windowWidth="30240" windowHeight="18880" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -18128,7 +18128,7 @@
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="29">
+  <cellXfs count="30">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
@@ -18198,6 +18198,7 @@
     <xf numFmtId="43" fontId="0" fillId="0" borderId="4" xfId="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="43" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="43" fontId="0" fillId="4" borderId="2" xfId="1" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="4">
     <cellStyle name="Check Cell" xfId="2" builtinId="23"/>
@@ -18483,8 +18484,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{46281658-57B8-5448-837E-93A14A80B5CE}">
   <dimension ref="A1:D2977"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D30" sqref="D30"/>
+    <sheetView tabSelected="1" topLeftCell="A895" workbookViewId="0">
+      <selection activeCell="B919" sqref="B919"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -32252,12 +32253,12 @@
       <c r="A918" s="1" t="s">
         <v>916</v>
       </c>
-      <c r="B918" s="3">
-        <v>1206500</v>
+      <c r="B918" s="29">
+        <v>1540400</v>
       </c>
       <c r="C918" s="27">
         <f t="shared" si="14"/>
-        <v>12065</v>
+        <v>15404</v>
       </c>
       <c r="D918" t="s">
         <v>3892</v>

</xml_diff>